<commit_message>
Updated the xlsx file, Nationokar school Data and maintained the app code
</commit_message>
<xml_diff>
--- a/School Enrolment&Attendance/Enrolment Data vs Attendance Report.xlsx
+++ b/School Enrolment&Attendance/Enrolment Data vs Attendance Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohnKul\Downloads\DSC-Johntrial\School Enrolment&amp;Attendance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5DA5EB-B11F-4D2F-9820-F48706933410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AB2553-5391-4F64-980D-A52FC346314E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="1" xr2:uid="{889C745F-092E-49DF-9274-E116BEDAB7D2}"/>
   </bookViews>
@@ -3135,18 +3135,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40EF40A3-FB82-4FAD-B863-9C82B855B50E}">
   <dimension ref="A1:I486"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M483" sqref="M483"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="N70" sqref="N70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
     <col min="5" max="5" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.36328125" customWidth="1"/>
+    <col min="8" max="8" width="7.453125" customWidth="1"/>
+    <col min="9" max="9" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -16348,9 +16348,15 @@
       <c r="A456" t="s">
         <v>20</v>
       </c>
-      <c r="B456" s="4"/>
-      <c r="C456" s="4"/>
-      <c r="D456" s="4"/>
+      <c r="B456" s="4">
+        <v>45.4</v>
+      </c>
+      <c r="C456" s="4">
+        <v>47.8</v>
+      </c>
+      <c r="D456" s="4">
+        <v>93.2</v>
+      </c>
       <c r="E456" s="1" t="s">
         <v>2</v>
       </c>
@@ -16371,9 +16377,15 @@
       <c r="A457" t="s">
         <v>20</v>
       </c>
-      <c r="B457" s="4"/>
-      <c r="C457" s="4"/>
-      <c r="D457" s="4"/>
+      <c r="B457" s="4">
+        <v>54.8</v>
+      </c>
+      <c r="C457" s="4">
+        <v>47.2</v>
+      </c>
+      <c r="D457" s="4">
+        <v>102</v>
+      </c>
       <c r="E457" s="1" t="s">
         <v>3</v>
       </c>
@@ -16394,9 +16406,15 @@
       <c r="A458" t="s">
         <v>20</v>
       </c>
-      <c r="B458" s="4"/>
-      <c r="C458" s="4"/>
-      <c r="D458" s="4"/>
+      <c r="B458" s="4">
+        <v>66.2</v>
+      </c>
+      <c r="C458" s="4">
+        <v>50</v>
+      </c>
+      <c r="D458" s="4">
+        <v>116.2</v>
+      </c>
       <c r="E458" s="1" t="s">
         <v>4</v>
       </c>
@@ -16417,9 +16435,15 @@
       <c r="A459" t="s">
         <v>20</v>
       </c>
-      <c r="B459" s="4"/>
-      <c r="C459" s="4"/>
-      <c r="D459" s="4"/>
+      <c r="B459" s="4">
+        <v>67.8</v>
+      </c>
+      <c r="C459" s="4">
+        <v>52.2</v>
+      </c>
+      <c r="D459" s="4">
+        <v>120</v>
+      </c>
       <c r="E459" s="1" t="s">
         <v>5</v>
       </c>
@@ -16440,9 +16464,15 @@
       <c r="A460" t="s">
         <v>20</v>
       </c>
-      <c r="B460" s="4"/>
-      <c r="C460" s="4"/>
-      <c r="D460" s="4"/>
+      <c r="B460" s="4">
+        <v>83</v>
+      </c>
+      <c r="C460" s="4">
+        <v>64</v>
+      </c>
+      <c r="D460" s="4">
+        <v>147</v>
+      </c>
       <c r="E460" s="1" t="s">
         <v>6</v>
       </c>
@@ -16463,9 +16493,15 @@
       <c r="A461" t="s">
         <v>20</v>
       </c>
-      <c r="B461" s="4"/>
-      <c r="C461" s="4"/>
-      <c r="D461" s="4"/>
+      <c r="B461" s="4">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="C461" s="4">
+        <v>57.4</v>
+      </c>
+      <c r="D461" s="4">
+        <v>139</v>
+      </c>
       <c r="E461" s="1" t="s">
         <v>7</v>
       </c>
@@ -16486,9 +16522,15 @@
       <c r="A462" t="s">
         <v>20</v>
       </c>
-      <c r="B462" s="4"/>
-      <c r="C462" s="4"/>
-      <c r="D462" s="4"/>
+      <c r="B462" s="4">
+        <v>63.6</v>
+      </c>
+      <c r="C462" s="4">
+        <v>57.2</v>
+      </c>
+      <c r="D462" s="4">
+        <v>120.8</v>
+      </c>
       <c r="E462" s="1" t="s">
         <v>8</v>
       </c>
@@ -16509,9 +16551,15 @@
       <c r="A463" t="s">
         <v>20</v>
       </c>
-      <c r="B463" s="4"/>
-      <c r="C463" s="4"/>
-      <c r="D463" s="4"/>
+      <c r="B463" s="4">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="C463" s="4">
+        <v>50.8</v>
+      </c>
+      <c r="D463" s="4">
+        <v>125.2</v>
+      </c>
       <c r="E463" s="1" t="s">
         <v>9</v>
       </c>
@@ -16532,9 +16580,15 @@
       <c r="A464" t="s">
         <v>20</v>
       </c>
-      <c r="B464" s="4"/>
-      <c r="C464" s="4"/>
-      <c r="D464" s="4"/>
+      <c r="B464" s="4">
+        <v>59.4</v>
+      </c>
+      <c r="C464" s="4">
+        <v>53.4</v>
+      </c>
+      <c r="D464" s="4">
+        <v>112.8</v>
+      </c>
       <c r="E464" s="1" t="s">
         <v>10</v>
       </c>
@@ -16555,9 +16609,15 @@
       <c r="A465" t="s">
         <v>20</v>
       </c>
-      <c r="B465" s="4"/>
-      <c r="C465" s="4"/>
-      <c r="D465" s="4"/>
+      <c r="B465" s="4">
+        <v>63.8</v>
+      </c>
+      <c r="C465" s="4">
+        <v>54.4</v>
+      </c>
+      <c r="D465" s="4">
+        <v>118.2</v>
+      </c>
       <c r="E465" s="1" t="s">
         <v>11</v>
       </c>
@@ -16578,9 +16638,15 @@
       <c r="A466" t="s">
         <v>20</v>
       </c>
-      <c r="B466" s="4"/>
-      <c r="C466" s="4"/>
-      <c r="D466" s="4"/>
+      <c r="B466" s="4">
+        <v>51</v>
+      </c>
+      <c r="C466" s="4">
+        <v>46.8</v>
+      </c>
+      <c r="D466" s="4">
+        <v>97.8</v>
+      </c>
       <c r="E466" s="1" t="s">
         <v>12</v>
       </c>

</xml_diff>